<commit_message>
feat: analysis business problems by excel and power bi
</commit_message>
<xml_diff>
--- a/Design/Sakila_Pivot_Analysis.xlsx
+++ b/Design/Sakila_Pivot_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Education\Uni\DataWarehouse\Final\Sakila-DataWarehouse\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB0D8DF-E37D-437F-8D31-933DF7F38FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34CF8D6-741B-45EB-BF55-98A97DE557A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{27116563-2158-4F54-A24E-7BA4B603F6CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{27116563-2158-4F54-A24E-7BA4B603F6CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Expense-Rental" sheetId="3" r:id="rId1"/>
@@ -18,9 +18,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId3"/>
-    <pivotCache cacheId="65" r:id="rId4"/>
-    <pivotCache cacheId="142" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -227,14 +227,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -247,20 +246,52 @@
   <dxfs count="52">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
       </font>
     </dxf>
     <dxf>
@@ -298,6 +329,81 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -317,6 +423,151 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -437,258 +688,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3040,6 +3039,706 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="24"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="25"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="26"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="27"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="28"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="29"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="30"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="31"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="32"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="33"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="34"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="35"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="36"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="37"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="38"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="39"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="40"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="41"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="42"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="43"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="44"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="45"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="46"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="47"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="48"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="49"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="50"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="51"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="52"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="53"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="54"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -3073,6 +3772,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3088,6 +3792,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3103,6 +3812,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3118,6 +3832,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -3133,6 +3852,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -3148,6 +3872,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -3165,6 +3894,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -3182,6 +3916,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -3199,6 +3938,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -3216,6 +3960,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -3328,6 +4077,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3343,6 +4097,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3358,6 +4117,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3373,6 +4137,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -3388,6 +4157,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -3403,6 +4177,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -3420,6 +4199,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -3437,6 +4221,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -3454,6 +4243,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -3471,6 +4265,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -3583,6 +4382,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3598,6 +4402,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3613,6 +4422,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3628,6 +4442,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -3643,6 +4462,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -3658,6 +4482,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -3675,6 +4504,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -3692,6 +4526,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -3709,6 +4548,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -3726,6 +4570,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -3838,6 +4687,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3853,6 +4707,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3868,6 +4727,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3883,6 +4747,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -3898,6 +4767,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000045-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -3913,6 +4787,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000047-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -3930,6 +4809,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000049-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -3947,6 +4831,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004B-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -3964,6 +4853,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004D-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -3981,6 +4875,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004F-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -4093,6 +4992,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000051-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4108,6 +5012,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000053-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -4123,6 +5032,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000055-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -4138,6 +5052,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000057-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -4153,6 +5072,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000059-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -4168,6 +5092,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005B-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -4185,6 +5114,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005D-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -4202,6 +5136,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005F-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -4219,6 +5158,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000061-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -4236,6 +5180,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000063-AF64-4665-B462-0D06F10CBF18}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -6046,6 +6995,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1880-4523-A7E9-760A8ECD942C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -6061,6 +7015,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1880-4523-A7E9-760A8ECD942C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -10177,7 +11136,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{98D678E2-EE3F-450C-826A-A4504FBF4941}" name="PivotTable2" cacheId="65" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{98D678E2-EE3F-450C-826A-A4504FBF4941}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
   <location ref="B24:H33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField allDrilled="1" subtotalTop="0" showAll="0" measureFilter="1" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -10272,54 +11231,57 @@
     <dataField fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="11">
-    <format dxfId="43">
+    <format dxfId="39">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="38">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="37">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="36">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="35">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="34">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="30">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="29">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <conditionalFormats count="13">
-    <conditionalFormat priority="13">
+    <conditionalFormat type="all" priority="1">
       <pivotAreas count="1">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
             <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="2" count="7">
@@ -10335,7 +11297,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="12">
+    <conditionalFormat type="all" priority="2">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -10343,7 +11305,7 @@
               <x v="0"/>
             </reference>
             <reference field="1" count="1" selected="0">
-              <x v="1"/>
+              <x v="0"/>
             </reference>
             <reference field="2" count="7">
               <x v="0"/>
@@ -10358,7 +11320,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="11">
+    <conditionalFormat type="all" priority="3">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -10366,7 +11328,7 @@
               <x v="0"/>
             </reference>
             <reference field="1" count="1" selected="0">
-              <x v="1"/>
+              <x v="4"/>
             </reference>
             <reference field="2" count="7">
               <x v="0"/>
@@ -10381,7 +11343,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="10">
+    <conditionalFormat type="all" priority="4">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -10389,7 +11351,7 @@
               <x v="0"/>
             </reference>
             <reference field="1" count="1" selected="0">
-              <x v="2"/>
+              <x v="4"/>
             </reference>
             <reference field="2" count="7">
               <x v="0"/>
@@ -10404,7 +11366,53 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="9">
+    <conditionalFormat type="all" priority="5">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="6">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="2" count="7">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat type="all" priority="7">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -10450,7 +11458,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="7">
+    <conditionalFormat type="all" priority="9">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -10473,7 +11481,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="6">
+    <conditionalFormat type="all" priority="10">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -10481,7 +11489,7 @@
               <x v="0"/>
             </reference>
             <reference field="1" count="1" selected="0">
-              <x v="3"/>
+              <x v="2"/>
             </reference>
             <reference field="2" count="7">
               <x v="0"/>
@@ -10496,7 +11504,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="5">
+    <conditionalFormat type="all" priority="11">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -10504,7 +11512,7 @@
               <x v="0"/>
             </reference>
             <reference field="1" count="1" selected="0">
-              <x v="3"/>
+              <x v="1"/>
             </reference>
             <reference field="2" count="7">
               <x v="0"/>
@@ -10519,7 +11527,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="4">
+    <conditionalFormat type="all" priority="12">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -10527,7 +11535,7 @@
               <x v="0"/>
             </reference>
             <reference field="1" count="1" selected="0">
-              <x v="4"/>
+              <x v="1"/>
             </reference>
             <reference field="2" count="7">
               <x v="0"/>
@@ -10542,60 +11550,11 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat type="all" priority="3">
+    <conditionalFormat priority="13">
       <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
             <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="2">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="7">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat type="all" priority="1">
-      <pivotAreas count="1">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="1" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="2" count="7">
@@ -10756,7 +11715,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E0BCB3F-52BE-43BD-BD55-F1668490D9F8}" name="PivotTable1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="18" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E0BCB3F-52BE-43BD-BD55-F1668490D9F8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="18" fieldListSortAscending="1">
   <location ref="B3:H15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -10849,42 +11808,42 @@
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="10">
-    <format dxfId="31">
+    <format dxfId="0">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="2">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="3">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="4">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="5">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -10913,7 +11872,7 @@
       </pivotAreas>
     </conditionalFormat>
   </conditionalFormats>
-  <chartFormats count="10">
+  <chartFormats count="60">
     <chartFormat chart="3" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -11027,6 +11986,756 @@
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="16">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="19">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="28">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="29">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="30">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="31">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="32">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="33">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="34">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="35">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="36">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="37">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="38">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="39">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="40">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="41">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="42">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="43">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="44">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="45">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="46">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="47">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="48">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="49">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="50">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="51">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="52">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="53">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="54">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="9"/>
           </reference>
           <reference field="2" count="1" selected="0">
             <x v="4"/>
@@ -11109,7 +12818,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1">
         <x14:conditionalFormats count="5">
-          <x14:conditionalFormat priority="24" id="{15745E97-9939-4517-8A04-29D4F9D687C5}">
+          <x14:conditionalFormat priority="20" id="{B63F468B-07FD-4255-908B-DD90BC519718}">
             <x14:pivotAreas count="1">
               <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
                 <references count="3">
@@ -11129,7 +12838,59 @@
                     <x v="9"/>
                   </reference>
                   <reference field="2" count="1" selected="0">
+                    <x v="4"/>
+                  </reference>
+                </references>
+              </pivotArea>
+            </x14:pivotAreas>
+          </x14:conditionalFormat>
+          <x14:conditionalFormat priority="21" id="{1D7458E5-6B23-4A90-A3E6-1C9739B17A2D}">
+            <x14:pivotAreas count="1">
+              <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+                <references count="3">
+                  <reference field="4294967294" count="1" selected="0">
                     <x v="0"/>
+                  </reference>
+                  <reference field="1" count="10">
+                    <x v="0"/>
+                    <x v="1"/>
+                    <x v="2"/>
+                    <x v="3"/>
+                    <x v="4"/>
+                    <x v="5"/>
+                    <x v="6"/>
+                    <x v="7"/>
+                    <x v="8"/>
+                    <x v="9"/>
+                  </reference>
+                  <reference field="2" count="1" selected="0">
+                    <x v="3"/>
+                  </reference>
+                </references>
+              </pivotArea>
+            </x14:pivotAreas>
+          </x14:conditionalFormat>
+          <x14:conditionalFormat priority="22" id="{16DD4843-82D4-4567-86B3-F15723CB8520}">
+            <x14:pivotAreas count="1">
+              <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+                <references count="3">
+                  <reference field="4294967294" count="1" selected="0">
+                    <x v="0"/>
+                  </reference>
+                  <reference field="1" count="10">
+                    <x v="0"/>
+                    <x v="1"/>
+                    <x v="2"/>
+                    <x v="3"/>
+                    <x v="4"/>
+                    <x v="5"/>
+                    <x v="6"/>
+                    <x v="7"/>
+                    <x v="8"/>
+                    <x v="9"/>
+                  </reference>
+                  <reference field="2" count="1" selected="0">
+                    <x v="2"/>
                   </reference>
                 </references>
               </pivotArea>
@@ -11161,7 +12922,7 @@
               </pivotArea>
             </x14:pivotAreas>
           </x14:conditionalFormat>
-          <x14:conditionalFormat priority="22" id="{16DD4843-82D4-4567-86B3-F15723CB8520}">
+          <x14:conditionalFormat priority="24" id="{15745E97-9939-4517-8A04-29D4F9D687C5}">
             <x14:pivotAreas count="1">
               <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
                 <references count="3">
@@ -11181,59 +12942,7 @@
                     <x v="9"/>
                   </reference>
                   <reference field="2" count="1" selected="0">
-                    <x v="2"/>
-                  </reference>
-                </references>
-              </pivotArea>
-            </x14:pivotAreas>
-          </x14:conditionalFormat>
-          <x14:conditionalFormat priority="21" id="{1D7458E5-6B23-4A90-A3E6-1C9739B17A2D}">
-            <x14:pivotAreas count="1">
-              <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-                <references count="3">
-                  <reference field="4294967294" count="1" selected="0">
                     <x v="0"/>
-                  </reference>
-                  <reference field="1" count="10">
-                    <x v="0"/>
-                    <x v="1"/>
-                    <x v="2"/>
-                    <x v="3"/>
-                    <x v="4"/>
-                    <x v="5"/>
-                    <x v="6"/>
-                    <x v="7"/>
-                    <x v="8"/>
-                    <x v="9"/>
-                  </reference>
-                  <reference field="2" count="1" selected="0">
-                    <x v="3"/>
-                  </reference>
-                </references>
-              </pivotArea>
-            </x14:pivotAreas>
-          </x14:conditionalFormat>
-          <x14:conditionalFormat priority="20" id="{B63F468B-07FD-4255-908B-DD90BC519718}">
-            <x14:pivotAreas count="1">
-              <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-                <references count="3">
-                  <reference field="4294967294" count="1" selected="0">
-                    <x v="0"/>
-                  </reference>
-                  <reference field="1" count="10">
-                    <x v="0"/>
-                    <x v="1"/>
-                    <x v="2"/>
-                    <x v="3"/>
-                    <x v="4"/>
-                    <x v="5"/>
-                    <x v="6"/>
-                    <x v="7"/>
-                    <x v="8"/>
-                    <x v="9"/>
-                  </reference>
-                  <reference field="2" count="1" selected="0">
-                    <x v="4"/>
                   </reference>
                 </references>
               </pivotArea>
@@ -11250,7 +12959,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EC0394B9-F61D-4DDA-BA25-5455E458E287}" name="PivotTable3" cacheId="142" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EC0394B9-F61D-4DDA-BA25-5455E458E287}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15" fieldListSortAscending="1">
   <location ref="B3:E17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -11339,7 +13048,7 @@
     <dataField fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="29">
+    <format dxfId="28">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -11348,39 +13057,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="27">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="28">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="27">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
     </format>
     <format dxfId="26">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="0"/>
@@ -11392,7 +13076,7 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="0"/>
@@ -11402,14 +13086,97 @@
       </pivotArea>
     </format>
     <format dxfId="24">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="21">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
   </formats>
   <conditionalFormats count="4">
-    <conditionalFormat priority="10">
+    <conditionalFormat priority="7">
+      <pivotAreas count="4">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="3" count="5">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="8">
       <pivotAreas count="4">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -11549,7 +13316,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="8">
+    <conditionalFormat priority="10">
       <pivotAreas count="4">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -11607,64 +13374,6 @@
             </reference>
             <reference field="1" count="1" selected="0">
               <x v="0"/>
-            </reference>
-            <reference field="3" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="7">
-      <pivotAreas count="4">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="3" count="5">
-              <x v="0"/>
-              <x v="1"/>
-              <x v="2"/>
-              <x v="3"/>
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="0" count="1" selected="0">
-              <x v="1"/>
             </reference>
             <reference field="3" count="5">
               <x v="0"/>
@@ -11778,13 +13487,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{54635CDB-36B2-4D32-BC3D-3B59FD62E736}" name="Table4" displayName="Table4" ref="B27:E33" totalsRowCount="1" headerRowDxfId="16" dataDxfId="17" headerRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{54635CDB-36B2-4D32-BC3D-3B59FD62E736}" name="Table4" displayName="Table4" ref="B27:E33" totalsRowCount="1" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
   <autoFilter ref="B27:E32" xr:uid="{54635CDB-36B2-4D32-BC3D-3B59FD62E736}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8500DC3C-C701-403A-9257-70D96E5535CE}" name="Month" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{776E815B-7758-40E2-A54A-B26203A1370B}" name="1" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{A3588CCD-68F4-439E-9566-A72EA12597C6}" name="2" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{2B539642-9B3B-483C-9EF7-9C00B333C0E7}" name="Quantity" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{8500DC3C-C701-403A-9257-70D96E5535CE}" name="Month" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{776E815B-7758-40E2-A54A-B26203A1370B}" name="1" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{A3588CCD-68F4-439E-9566-A72EA12597C6}" name="2" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{2B539642-9B3B-483C-9EF7-9C00B333C0E7}" name="Quantity" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12109,8 +13818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBBA9D3-0048-4D30-8DE7-49F83EE6D522}">
   <dimension ref="A2:I151"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27:Y27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12383,22 +14092,22 @@
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <v>7</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1">
         <v>50</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="1">
         <v>113</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="1">
         <v>319</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="1">
         <v>259</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="1">
         <v>748</v>
       </c>
       <c r="I5" s="1"/>
@@ -12408,22 +14117,22 @@
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="1">
         <v>13</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>109</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>198</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="1">
         <v>594</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>512</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>1426</v>
       </c>
       <c r="I6" s="1"/>
@@ -12433,22 +14142,22 @@
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>23</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>111</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>208</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="1">
         <v>651</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>579</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
         <v>1572</v>
       </c>
       <c r="I7" s="1"/>
@@ -12458,22 +14167,22 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>31</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>58</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>139</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>137</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>367</v>
       </c>
       <c r="I8" s="1"/>
@@ -12483,22 +14192,22 @@
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="1">
         <v>9</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>65</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <v>117</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="1">
         <v>334</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>300</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="1">
         <v>825</v>
       </c>
       <c r="I9" s="1"/>
@@ -12508,22 +14217,22 @@
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>6</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>63</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>117</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="1">
         <v>320</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>290</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="1">
         <v>796</v>
       </c>
       <c r="I10" s="1"/>
@@ -12533,22 +14242,22 @@
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="1">
         <v>38</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>83</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="1">
         <v>232</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <v>205</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="1">
         <v>568</v>
       </c>
       <c r="I11" s="1"/>
@@ -12558,22 +14267,22 @@
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="1">
         <v>60</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="1">
         <v>106</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>308</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <v>235</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="1">
         <v>713</v>
       </c>
       <c r="I12" s="1"/>
@@ -12583,22 +14292,22 @@
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="1">
         <v>3</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="1">
         <v>27</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="1">
         <v>52</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="1">
         <v>172</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="1">
         <v>134</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="1">
         <v>388</v>
       </c>
       <c r="I13" s="1"/>
@@ -12608,22 +14317,22 @@
       <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="1">
         <v>11</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="1">
         <v>70</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="1">
         <v>152</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="1">
         <v>376</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="1">
         <v>359</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="1">
         <v>968</v>
       </c>
       <c r="I14" s="1"/>
@@ -12633,22 +14342,22 @@
       <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="1">
         <v>88</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="1">
         <v>624</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="1">
         <v>1204</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="1">
         <v>3445</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="1">
         <v>3010</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="1">
         <v>8371</v>
       </c>
       <c r="I15" s="1"/>
@@ -12726,20 +14435,20 @@
       <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4">
         <v>472</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <v>1057</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <v>1482</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>4110</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="4">
         <v>7121</v>
       </c>
     </row>
@@ -12747,22 +14456,22 @@
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>358</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="4">
         <v>561</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="4">
         <v>931</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="4">
         <v>1845</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <v>4108</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="4">
         <v>7803</v>
       </c>
     </row>
@@ -12770,20 +14479,20 @@
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4">
         <v>438</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <v>1032</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="4">
         <v>3717</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <v>1870</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="4">
         <v>7057</v>
       </c>
     </row>
@@ -12791,20 +14500,20 @@
       <c r="B29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4">
         <v>582</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <v>1029</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="4">
         <v>3451</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <v>2096</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="4">
         <v>7158</v>
       </c>
     </row>
@@ -12812,20 +14521,20 @@
       <c r="B30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4">
         <v>520</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="4">
         <v>1011</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="4">
         <v>3791</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="4">
         <v>1994</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="4">
         <v>7316</v>
       </c>
     </row>
@@ -12833,20 +14542,20 @@
       <c r="B31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4">
         <v>610</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="4">
         <v>1146</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="4">
         <v>3781</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="4">
         <v>2106</v>
       </c>
-      <c r="H31" s="5">
+      <c r="H31" s="4">
         <v>7643</v>
       </c>
     </row>
@@ -12854,20 +14563,20 @@
       <c r="B32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5">
+      <c r="C32" s="4"/>
+      <c r="D32" s="4">
         <v>496</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="4">
         <v>1136</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="4">
         <v>3660</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="4">
         <v>2157</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="4">
         <v>7449</v>
       </c>
     </row>
@@ -12875,22 +14584,22 @@
       <c r="B33" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <v>358</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="4">
         <v>3679</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="4">
         <v>7342</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="4">
         <v>21727</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="4">
         <v>18441</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H33" s="4">
         <v>51547</v>
       </c>
     </row>
@@ -12903,109 +14612,6 @@
     <row r="40" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
     <row r="41" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
     <row r="42" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="2:8" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="68" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="69" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="74" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="77" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="82" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="83" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="85" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="86" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="87" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="88" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="89" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="90" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="91" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="92" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="93" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="94" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="95" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="96" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="97" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="98" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="99" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="100" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="101" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="102" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="103" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="104" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="105" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="106" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="107" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="108" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="109" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="110" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="111" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="112" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="113" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="114" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="115" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="116" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="117" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="118" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="119" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="120" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="121" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="122" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="123" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="124" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="125" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="126" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="127" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="128" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="129" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="130" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="131" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="132" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="133" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="134" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="135" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="136" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="137" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="138" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="139" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="140" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="141" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="142" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="143" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="144" ht="18" x14ac:dyDescent="0.35"/>
-    <row r="145" ht="18" x14ac:dyDescent="0.35"/>
     <row r="151" ht="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="C2">
@@ -13047,40 +14653,40 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="D26:D32">
-    <cfRule type="top10" dxfId="15" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="51" priority="12" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="D26:D32">
-    <cfRule type="top10" dxfId="14" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="50" priority="11" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="E26:E32">
-    <cfRule type="top10" dxfId="13" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="49" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="E26:E32">
-    <cfRule type="top10" dxfId="12" priority="9" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="48" priority="9" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="D26:D32">
-    <cfRule type="top10" dxfId="11" priority="8" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="47" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="E26:E32">
-    <cfRule type="top10" dxfId="10" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="46" priority="7" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="F26:F32">
-    <cfRule type="top10" dxfId="9" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="45" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="F26:F32">
-    <cfRule type="top10" dxfId="8" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="44" priority="5" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="G26:G32">
-    <cfRule type="top10" dxfId="7" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="43" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="G26:G32">
-    <cfRule type="top10" dxfId="6" priority="3" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="42" priority="3" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="C26:C32">
-    <cfRule type="top10" dxfId="5" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="41" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="C26:C32">
-    <cfRule type="top10" dxfId="4" priority="1" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="40" priority="1" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>
@@ -13099,6 +14705,19 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>C2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
+          <x14:cfRule type="dataBar" id="{B91289AB-41AA-4444-9EBF-09B700301D4E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H26:H32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
           <x14:cfRule type="iconSet" priority="24" id="{15745E97-9939-4517-8A04-29D4F9D687C5}">
@@ -13180,36 +14799,23 @@
           </x14:cfRule>
           <xm:sqref>G5:G14</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
-          <x14:cfRule type="dataBar" id="{B91289AB-41AA-4444-9EBF-09B700301D4E}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FFFFB628"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H26:H32</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{E89A34F7-DB47-4450-B6CD-C17BF777A42E}">
-          <x14:colorSeries theme="5"/>
-          <x14:colorNegative theme="6"/>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{1CF6F669-2EBC-4810-8AE3-F27377EC7C36}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="5" tint="-0.249977111117893"/>
-          <x14:colorFirst theme="5" tint="-0.249977111117893"/>
-          <x14:colorLast theme="5" tint="-0.249977111117893"/>
-          <x14:colorHigh theme="5" tint="-0.249977111117893"/>
-          <x14:colorLow theme="5" tint="-0.249977111117893"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Expense-Rental'!P4:P111</xm:f>
-              <xm:sqref>P112</xm:sqref>
+              <xm:f>'Expense-Rental'!H5:H14</xm:f>
+              <xm:sqref>H15</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -13249,19 +14855,19 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{1CF6F669-2EBC-4810-8AE3-F27377EC7C36}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" high="1" low="1" xr2:uid="{E89A34F7-DB47-4450-B6CD-C17BF777A42E}">
+          <x14:colorSeries theme="5"/>
+          <x14:colorNegative theme="6"/>
           <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
+          <x14:colorMarkers theme="5" tint="-0.249977111117893"/>
+          <x14:colorFirst theme="5" tint="-0.249977111117893"/>
+          <x14:colorLast theme="5" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="5" tint="-0.249977111117893"/>
+          <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Expense-Rental'!H5:H14</xm:f>
-              <xm:sqref>H15</xm:sqref>
+              <xm:f>'Expense-Rental'!P4:P111</xm:f>
+              <xm:sqref>P112</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -13275,7 +14881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93263BDF-1496-4A52-9C4A-10BE87CFB5D0}">
   <dimension ref="B3:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -13323,67 +14929,67 @@
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
         <v>146</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>146</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1788</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4">
         <v>1788</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>3681</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4">
         <v>3681</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>10753</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4">
         <v>10753</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>9209</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
         <v>9209</v>
       </c>
     </row>
@@ -13391,67 +14997,67 @@
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4">
         <v>212</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>212</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>1891</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4">
         <v>1891</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>3661</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4">
         <v>3661</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>10974</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4">
         <v>10974</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>9232</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4">
         <v>9232</v>
       </c>
     </row>
@@ -13459,30 +15065,30 @@
       <c r="B17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>51189</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>358</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>51547</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B25" s="5"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="27" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -13490,13 +15096,13 @@
       <c r="B28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="1">
         <v>85</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="1">
         <v>97</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="1">
         <v>182</v>
       </c>
     </row>
@@ -13504,13 +15110,13 @@
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="1">
         <v>558</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="1">
         <v>598</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="1">
         <v>1156</v>
       </c>
     </row>
@@ -13518,13 +15124,13 @@
       <c r="B30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="1">
         <v>1163</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="1">
         <v>1148</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="1">
         <v>2311</v>
       </c>
     </row>
@@ -13532,13 +15138,13 @@
       <c r="B31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="1">
         <v>3342</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="1">
         <v>3367</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="1">
         <v>6709</v>
       </c>
     </row>
@@ -13546,13 +15152,13 @@
       <c r="B32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="1">
         <v>2892</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="1">
         <v>2794</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="1">
         <v>5686</v>
       </c>
     </row>

</xml_diff>